<commit_message>
testData function for the xlsx's in nmadb
</commit_message>
<xml_diff>
--- a/nmadb/479531.xlsx
+++ b/nmadb/479531.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,9 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$58</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet2!$A$1:$B$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$58</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$F$58</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet2!$A$1:$B$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet2!$A$1:$B$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="60">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -39,7 +41,7 @@
     <t xml:space="preserve">id</t>
   </si>
   <si>
-    <t xml:space="preserve">tx</t>
+    <t xml:space="preserve">t</t>
   </si>
   <si>
     <t xml:space="preserve">r</t>
@@ -341,9 +343,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -354,15 +360,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -442,7 +440,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -475,7 +473,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFDEADA"/>
+      <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -509,7 +507,7 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFE6E0EC"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFFDEADA"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
@@ -550,41 +548,41 @@
   </sheetPr>
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="2" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -595,32 +593,34 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="2" t="n">
         <v>71</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="2" t="n">
         <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
-      <c r="C3" s="1" t="n">
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>73</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="2" t="n">
         <v>105</v>
       </c>
     </row>
@@ -631,32 +631,34 @@
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E4" s="6" t="n">
         <v>173</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="2" t="n">
         <v>254</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
-      <c r="B5" s="0"/>
-      <c r="C5" s="1" t="n">
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="6" t="n">
         <v>196</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" s="2" t="n">
         <v>255</v>
       </c>
     </row>
@@ -667,32 +669,34 @@
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="6" t="n">
         <v>177</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="F6" s="2" t="n">
         <v>212</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
-      <c r="B7" s="0"/>
-      <c r="C7" s="1" t="n">
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="E7" s="6" t="n">
         <v>165</v>
       </c>
-      <c r="F7" s="1" t="n">
+      <c r="F7" s="2" t="n">
         <v>217</v>
       </c>
     </row>
@@ -703,32 +707,34 @@
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="2" t="n">
         <v>44</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="F8" s="2" t="n">
         <v>53</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0"/>
-      <c r="B9" s="0"/>
-      <c r="C9" s="1" t="n">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="F9" s="1" t="n">
+      <c r="F9" s="2" t="n">
         <v>53</v>
       </c>
     </row>
@@ -739,32 +745,34 @@
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="2" t="n">
         <v>97</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="F10" s="2" t="n">
         <v>114</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
-      <c r="B11" s="0"/>
-      <c r="C11" s="1" t="n">
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="2" t="n">
         <v>93</v>
       </c>
-      <c r="F11" s="1" t="n">
+      <c r="F11" s="2" t="n">
         <v>105</v>
       </c>
     </row>
@@ -775,32 +783,34 @@
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="E12" s="4" t="n">
+      <c r="E12" s="6" t="n">
         <v>276</v>
       </c>
-      <c r="F12" s="1" t="n">
+      <c r="F12" s="2" t="n">
         <v>346</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
-      <c r="B13" s="0"/>
-      <c r="C13" s="1" t="n">
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="E13" s="4" t="n">
+      <c r="E13" s="6" t="n">
         <v>287</v>
       </c>
-      <c r="F13" s="1" t="n">
+      <c r="F13" s="2" t="n">
         <v>343</v>
       </c>
     </row>
@@ -811,32 +821,34 @@
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="D14" s="3" t="n">
+      <c r="D14" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="E14" s="4" t="n">
+      <c r="E14" s="6" t="n">
         <v>114</v>
       </c>
-      <c r="F14" s="1" t="n">
+      <c r="F14" s="2" t="n">
         <v>192</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0"/>
-      <c r="B15" s="0"/>
-      <c r="C15" s="1" t="n">
+      <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="E15" s="4" t="n">
+      <c r="E15" s="6" t="n">
         <v>137</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="F15" s="2" t="n">
         <v>193</v>
       </c>
     </row>
@@ -847,32 +859,34 @@
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="1" t="n">
+      <c r="C16" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="D16" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="E16" s="4" t="n">
+      <c r="E16" s="6" t="n">
         <v>48</v>
       </c>
-      <c r="F16" s="1" t="n">
+      <c r="F16" s="2" t="n">
         <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
-      <c r="B17" s="0"/>
-      <c r="C17" s="1" t="n">
+      <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="E17" s="4" t="n">
+      <c r="E17" s="6" t="n">
         <v>43</v>
       </c>
-      <c r="F17" s="1" t="n">
+      <c r="F17" s="2" t="n">
         <v>57</v>
       </c>
     </row>
@@ -883,32 +897,34 @@
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="1" t="n">
+      <c r="C18" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="E18" s="4" t="n">
+      <c r="E18" s="6" t="n">
         <v>343</v>
       </c>
-      <c r="F18" s="1" t="n">
+      <c r="F18" s="2" t="n">
         <v>440</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0"/>
-      <c r="B19" s="0"/>
-      <c r="C19" s="1" t="n">
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="E19" s="4" t="n">
+      <c r="E19" s="6" t="n">
         <v>338</v>
       </c>
-      <c r="F19" s="1" t="n">
+      <c r="F19" s="2" t="n">
         <v>443</v>
       </c>
     </row>
@@ -919,68 +935,71 @@
       <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="1" t="n">
+      <c r="C20" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D20" s="3" t="n">
+      <c r="D20" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="E20" s="4" t="n">
+      <c r="E20" s="6" t="n">
         <v>73</v>
       </c>
-      <c r="F20" s="1" t="n">
+      <c r="F20" s="2" t="n">
         <v>97</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0"/>
-      <c r="B21" s="0"/>
-      <c r="C21" s="1" t="n">
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="E21" s="2" t="n">
         <v>57</v>
       </c>
-      <c r="F21" s="1" t="n">
+      <c r="F21" s="2" t="n">
         <v>96</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="n">
+      <c r="A22" s="1" t="n">
         <v>2004</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="5" t="n">
+      <c r="C22" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="D22" s="6" t="n">
+      <c r="D22" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="E22" s="7" t="n">
+      <c r="E22" s="6" t="n">
         <v>226</v>
       </c>
-      <c r="F22" s="5" t="n">
+      <c r="F22" s="2" t="n">
         <v>324</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5" t="n">
+      <c r="B23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="D23" s="6" t="n">
+      <c r="D23" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="E23" s="7" t="n">
+      <c r="E23" s="6" t="n">
         <v>224</v>
       </c>
-      <c r="F23" s="5" t="n">
+      <c r="F23" s="2" t="n">
         <v>325</v>
       </c>
     </row>
@@ -991,32 +1010,34 @@
       <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="1" t="n">
+      <c r="C24" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="D24" s="1" t="n">
+      <c r="D24" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="E24" s="4" t="n">
+      <c r="E24" s="6" t="n">
         <v>281</v>
       </c>
-      <c r="F24" s="1" t="n">
+      <c r="F24" s="2" t="n">
         <v>344</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
-      <c r="B25" s="0"/>
-      <c r="C25" s="1" t="n">
+      <c r="B25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="D25" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="E25" s="4" t="n">
+      <c r="E25" s="6" t="n">
         <v>285</v>
       </c>
-      <c r="F25" s="1" t="n">
+      <c r="F25" s="2" t="n">
         <v>346</v>
       </c>
     </row>
@@ -1027,64 +1048,70 @@
       <c r="B26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="1" t="n">
+      <c r="C26" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="D26" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="E26" s="4" t="n">
+      <c r="E26" s="6" t="n">
         <v>68</v>
       </c>
-      <c r="F26" s="1" t="n">
+      <c r="F26" s="2" t="n">
         <v>80</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
-      <c r="B27" s="0"/>
-      <c r="C27" s="1" t="n">
+      <c r="B27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="D27" s="1" t="n">
+      <c r="D27" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="E27" s="1" t="n">
+      <c r="E27" s="2" t="n">
         <v>132</v>
       </c>
-      <c r="F27" s="1" t="n">
+      <c r="F27" s="2" t="n">
         <v>162</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
-      <c r="B28" s="0"/>
-      <c r="C28" s="1" t="n">
+      <c r="B28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="D28" s="1" t="n">
+      <c r="D28" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="E28" s="1" t="n">
+      <c r="E28" s="2" t="n">
         <v>71</v>
       </c>
-      <c r="F28" s="1" t="n">
+      <c r="F28" s="2" t="n">
         <v>79</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
-      <c r="B29" s="0"/>
-      <c r="C29" s="1" t="n">
+      <c r="B29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="D29" s="1" t="n">
+      <c r="D29" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="E29" s="1" t="n">
+      <c r="E29" s="2" t="n">
         <v>146</v>
       </c>
-      <c r="F29" s="1" t="n">
+      <c r="F29" s="2" t="n">
         <v>163</v>
       </c>
     </row>
@@ -1095,32 +1122,34 @@
       <c r="B30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="1" t="n">
+      <c r="C30" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="D30" s="1" t="n">
+      <c r="D30" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="E30" s="1" t="n">
+      <c r="E30" s="2" t="n">
         <v>296</v>
       </c>
-      <c r="F30" s="1" t="n">
+      <c r="F30" s="2" t="n">
         <v>352</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
-      <c r="B31" s="0"/>
-      <c r="C31" s="1" t="n">
+      <c r="B31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="D31" s="1" t="n">
+      <c r="D31" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="E31" s="1" t="n">
+      <c r="E31" s="2" t="n">
         <v>305</v>
       </c>
-      <c r="F31" s="1" t="n">
+      <c r="F31" s="2" t="n">
         <v>348</v>
       </c>
     </row>
@@ -1131,32 +1160,34 @@
       <c r="B32" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="1" t="n">
+      <c r="C32" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="D32" s="1" t="n">
+      <c r="D32" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="E32" s="1" t="n">
+      <c r="E32" s="2" t="n">
         <v>308</v>
       </c>
-      <c r="F32" s="1" t="n">
+      <c r="F32" s="2" t="n">
         <v>355</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="0"/>
-      <c r="C33" s="1" t="n">
+      <c r="B33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="D33" s="1" t="n">
+      <c r="D33" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="E33" s="1" t="n">
+      <c r="E33" s="2" t="n">
         <v>316</v>
       </c>
-      <c r="F33" s="1" t="n">
+      <c r="F33" s="2" t="n">
         <v>353</v>
       </c>
     </row>
@@ -1167,32 +1198,34 @@
       <c r="B34" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="1" t="n">
+      <c r="C34" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="D34" s="1" t="n">
+      <c r="D34" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="E34" s="1" t="n">
+      <c r="E34" s="2" t="n">
         <v>210</v>
       </c>
-      <c r="F34" s="1" t="n">
+      <c r="F34" s="2" t="n">
         <v>345</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
-      <c r="B35" s="0"/>
-      <c r="C35" s="1" t="n">
+      <c r="B35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="D35" s="1" t="n">
+      <c r="D35" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E35" s="1" t="n">
+      <c r="E35" s="2" t="n">
         <v>216</v>
       </c>
-      <c r="F35" s="1" t="n">
+      <c r="F35" s="2" t="n">
         <v>343</v>
       </c>
     </row>
@@ -1203,32 +1236,34 @@
       <c r="B36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="1" t="n">
+      <c r="C36" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="D36" s="1" t="n">
+      <c r="D36" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="E36" s="1" t="n">
+      <c r="E36" s="2" t="n">
         <v>288</v>
       </c>
-      <c r="F36" s="1" t="n">
+      <c r="F36" s="2" t="n">
         <v>444</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0"/>
-      <c r="B37" s="0"/>
-      <c r="C37" s="1" t="n">
+      <c r="B37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="D37" s="1" t="n">
+      <c r="D37" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E37" s="1" t="n">
+      <c r="E37" s="2" t="n">
         <v>285</v>
       </c>
-      <c r="F37" s="1" t="n">
+      <c r="F37" s="2" t="n">
         <v>434</v>
       </c>
     </row>
@@ -1239,32 +1274,34 @@
       <c r="B38" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="1" t="n">
+      <c r="C38" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="D38" s="3" t="n">
+      <c r="D38" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="E38" s="1" t="n">
+      <c r="E38" s="2" t="n">
         <v>36</v>
       </c>
-      <c r="F38" s="1" t="n">
+      <c r="F38" s="2" t="n">
         <v>63</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0"/>
-      <c r="B39" s="0"/>
-      <c r="C39" s="1" t="n">
+      <c r="B39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="D39" s="1" t="n">
+      <c r="D39" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E39" s="1" t="n">
+      <c r="E39" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="F39" s="1" t="n">
+      <c r="F39" s="2" t="n">
         <v>63</v>
       </c>
     </row>
@@ -1275,32 +1312,34 @@
       <c r="B40" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="1" t="n">
+      <c r="C40" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="D40" s="1" t="n">
+      <c r="D40" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="E40" s="1" t="n">
+      <c r="E40" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="F40" s="1" t="n">
+      <c r="F40" s="2" t="n">
         <v>77</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0"/>
-      <c r="B41" s="0"/>
-      <c r="C41" s="1" t="n">
+      <c r="B41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="D41" s="1" t="n">
+      <c r="D41" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="E41" s="1" t="n">
+      <c r="E41" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="F41" s="1" t="n">
+      <c r="F41" s="2" t="n">
         <v>75</v>
       </c>
     </row>
@@ -1311,48 +1350,52 @@
       <c r="B42" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="1" t="n">
+      <c r="C42" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D42" s="1" t="n">
+      <c r="D42" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="E42" s="1" t="n">
+      <c r="E42" s="2" t="n">
         <v>62</v>
       </c>
-      <c r="F42" s="1" t="n">
+      <c r="F42" s="2" t="n">
         <v>77</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0"/>
-      <c r="B43" s="0"/>
-      <c r="C43" s="1" t="n">
+      <c r="B43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D43" s="1" t="n">
+      <c r="D43" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="E43" s="1" t="n">
+      <c r="E43" s="2" t="n">
         <v>54</v>
       </c>
-      <c r="F43" s="1" t="n">
+      <c r="F43" s="2" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0"/>
-      <c r="B44" s="0"/>
-      <c r="C44" s="1" t="n">
+      <c r="B44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D44" s="1" t="n">
+      <c r="D44" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="E44" s="1" t="n">
+      <c r="E44" s="2" t="n">
         <v>56</v>
       </c>
-      <c r="F44" s="1" t="n">
+      <c r="F44" s="2" t="n">
         <v>81</v>
       </c>
     </row>
@@ -1363,32 +1406,34 @@
       <c r="B45" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C45" s="1" t="n">
+      <c r="C45" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="D45" s="1" t="n">
+      <c r="D45" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="E45" s="1" t="n">
+      <c r="E45" s="2" t="n">
         <v>338</v>
       </c>
-      <c r="F45" s="1" t="n">
+      <c r="F45" s="2" t="n">
         <v>419</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
-      <c r="B46" s="0"/>
-      <c r="C46" s="1" t="n">
+      <c r="B46" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="D46" s="1" t="n">
+      <c r="D46" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="E46" s="1" t="n">
+      <c r="E46" s="2" t="n">
         <v>364</v>
       </c>
-      <c r="F46" s="1" t="n">
+      <c r="F46" s="2" t="n">
         <v>414</v>
       </c>
     </row>
@@ -1399,64 +1444,70 @@
       <c r="B47" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C47" s="1" t="n">
+      <c r="C47" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="D47" s="1" t="n">
+      <c r="D47" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="E47" s="1" t="n">
+      <c r="E47" s="2" t="n">
         <v>145</v>
       </c>
-      <c r="F47" s="1" t="n">
+      <c r="F47" s="2" t="n">
         <v>169</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0"/>
-      <c r="B48" s="0"/>
-      <c r="C48" s="1" t="n">
+      <c r="B48" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="D48" s="1" t="n">
+      <c r="D48" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="E48" s="1" t="n">
+      <c r="E48" s="2" t="n">
         <v>216</v>
       </c>
-      <c r="F48" s="1" t="n">
+      <c r="F48" s="2" t="n">
         <v>242</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
-      <c r="B49" s="0"/>
-      <c r="C49" s="1" t="n">
+      <c r="B49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="D49" s="1" t="n">
+      <c r="D49" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="E49" s="1" t="n">
+      <c r="E49" s="2" t="n">
         <v>142</v>
       </c>
-      <c r="F49" s="1" t="n">
+      <c r="F49" s="2" t="n">
         <v>164</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
-      <c r="B50" s="0"/>
-      <c r="C50" s="1" t="n">
+      <c r="B50" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="D50" s="1" t="n">
+      <c r="D50" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="E50" s="1" t="n">
+      <c r="E50" s="2" t="n">
         <v>209</v>
       </c>
-      <c r="F50" s="1" t="n">
+      <c r="F50" s="2" t="n">
         <v>247</v>
       </c>
     </row>
@@ -1467,32 +1518,34 @@
       <c r="B51" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C51" s="1" t="n">
+      <c r="C51" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="D51" s="3" t="n">
+      <c r="D51" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="E51" s="1" t="n">
+      <c r="E51" s="2" t="n">
         <v>150</v>
       </c>
-      <c r="F51" s="1" t="n">
+      <c r="F51" s="2" t="n">
         <v>401</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0"/>
-      <c r="B52" s="0"/>
-      <c r="C52" s="1" t="n">
+      <c r="B52" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="D52" s="1" t="n">
+      <c r="D52" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E52" s="1" t="n">
+      <c r="E52" s="2" t="n">
         <v>131</v>
       </c>
-      <c r="F52" s="1" t="n">
+      <c r="F52" s="2" t="n">
         <v>404</v>
       </c>
     </row>
@@ -1503,32 +1556,34 @@
       <c r="B53" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C53" s="1" t="n">
+      <c r="C53" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="D53" s="1" t="n">
+      <c r="D53" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="E53" s="1" t="n">
+      <c r="E53" s="2" t="n">
         <v>320</v>
       </c>
-      <c r="F53" s="1" t="n">
+      <c r="F53" s="2" t="n">
         <v>392</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0"/>
-      <c r="B54" s="0"/>
-      <c r="C54" s="1" t="n">
+      <c r="B54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="D54" s="1" t="n">
+      <c r="D54" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="E54" s="1" t="n">
+      <c r="E54" s="2" t="n">
         <v>338</v>
       </c>
-      <c r="F54" s="1" t="n">
+      <c r="F54" s="2" t="n">
         <v>394</v>
       </c>
     </row>
@@ -1539,32 +1594,34 @@
       <c r="B55" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C55" s="1" t="n">
+      <c r="C55" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="D55" s="1" t="n">
+      <c r="D55" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="E55" s="1" t="n">
+      <c r="E55" s="2" t="n">
         <v>230</v>
       </c>
-      <c r="F55" s="1" t="n">
+      <c r="F55" s="2" t="n">
         <v>281</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0"/>
-      <c r="B56" s="0"/>
-      <c r="C56" s="1" t="n">
+      <c r="B56" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C56" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="D56" s="1" t="n">
+      <c r="D56" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="E56" s="1" t="n">
+      <c r="E56" s="2" t="n">
         <v>241</v>
       </c>
-      <c r="F56" s="1" t="n">
+      <c r="F56" s="2" t="n">
         <v>280</v>
       </c>
     </row>
@@ -1575,30 +1632,33 @@
       <c r="B57" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C57" s="1" t="n">
+      <c r="C57" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="D57" s="1" t="n">
+      <c r="D57" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="E57" s="1" t="n">
+      <c r="E57" s="2" t="n">
         <v>276</v>
       </c>
-      <c r="F57" s="1" t="n">
+      <c r="F57" s="2" t="n">
         <v>338</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="1" t="n">
+      <c r="B58" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C58" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="D58" s="1" t="n">
+      <c r="D58" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="E58" s="1" t="n">
+      <c r="E58" s="2" t="n">
         <v>291</v>
       </c>
-      <c r="F58" s="1" t="n">
+      <c r="F58" s="2" t="n">
         <v>340</v>
       </c>
     </row>
@@ -1622,229 +1682,229 @@
   </sheetPr>
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="11" t="n">
+      <c r="B2" s="10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="11" t="n">
+      <c r="B3" s="10" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="11" t="n">
+      <c r="B4" s="10" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="11" t="n">
+      <c r="B5" s="10" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="11" t="n">
+      <c r="B6" s="10" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="11" t="n">
+      <c r="B7" s="10" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="11" t="n">
+      <c r="B8" s="10" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="11" t="n">
+      <c r="B9" s="10" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="11" t="n">
+      <c r="B10" s="10" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="11" t="n">
+      <c r="B11" s="10" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="11" t="n">
+      <c r="B12" s="10" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="11" t="n">
+      <c r="B13" s="10" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="11" t="n">
+      <c r="B14" s="10" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="11" t="n">
+      <c r="B15" s="10" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="11" t="n">
+      <c r="B16" s="10" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="11" t="n">
+      <c r="B17" s="10" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="11" t="n">
+      <c r="B18" s="10" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="11" t="n">
+      <c r="B19" s="10" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="11" t="n">
+      <c r="B20" s="10" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="11" t="n">
+      <c r="B21" s="10" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="11" t="n">
+      <c r="B22" s="10" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="11" t="n">
+      <c r="B23" s="10" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="11" t="n">
+      <c r="B24" s="10" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="11" t="n">
+      <c r="B25" s="10" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="11" t="n">
+      <c r="B26" s="10" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="11" t="n">
+      <c r="B27" s="10" t="n">
         <v>12</v>
       </c>
     </row>
@@ -1884,17 +1944,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="14"/>
+      <c r="C1" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>